<commit_message>
first working chart example
</commit_message>
<xml_diff>
--- a/data/altersverteilung.xlsx
+++ b/data/altersverteilung.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\visual_storytelling\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programming\Others\visual_storytelling\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{431CA959-E5D6-4199-8872-4FE9D1F8C7EA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C25D9B25-6E16-46DD-9CDF-0212D702DD2D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16200" yWindow="3330" windowWidth="13395" windowHeight="9360" xr2:uid="{057F5124-1E2A-4AE4-842D-56B0C8C3042D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{057F5124-1E2A-4AE4-842D-56B0C8C3042D}"/>
   </bookViews>
   <sheets>
     <sheet name="altersverteilung" sheetId="1" r:id="rId1"/>
@@ -31,15 +31,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>Menge</t>
   </si>
   <si>
     <t>Alter</t>
-  </si>
-  <si>
-    <t>-</t>
   </si>
 </sst>
 </file>
@@ -393,8 +390,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00167490-1020-47F6-9D2D-50169C0DD28E}">
   <dimension ref="A1:B57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B58" sqref="B58"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -419,16 +416,16 @@
       <c r="A3">
         <v>11</v>
       </c>
-      <c r="B3" t="s">
-        <v>2</v>
+      <c r="B3">
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>12</v>
       </c>
-      <c r="B4" t="s">
-        <v>2</v>
+      <c r="B4">
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>